<commit_message>
update: rename column header name of dataset
</commit_message>
<xml_diff>
--- a/detectors/agg/dataset/dataset.xlsx
+++ b/detectors/agg/dataset/dataset.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pras\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\codes\nl2sql\detectors\agg\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74A33AB6-F271-4B83-ACD4-20E737108025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8621B7A4-F0F1-4468-B5D0-ADE25DD9F2DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{2F81A05F-9ACD-4458-AAFF-AD5E40FA328F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -5547,7 +5550,7 @@
   <dimension ref="A1:E841"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18177,6 +18180,7 @@
       <c r="E841" s="4"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E1" xr:uid="{8532AB5B-1DD6-4F7E-B08A-D1A13596D5DF}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>